<commit_message>
Chỉnh sửa lại store và Data input của danh muc địa điểm
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Danh muc dia diem/CF0141_Danh muc dia diem.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Danh muc dia diem/CF0141_Danh muc dia diem.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="15480" windowHeight="9990" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Update History" sheetId="4" r:id="rId1"/>
@@ -1327,7 +1327,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="293">
   <si>
     <t>Detail Design</t>
   </si>
@@ -2400,6 +2400,14 @@
   </si>
   <si>
     <t>Click System</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT CT41.StationID, CT41.[Address], CT41.StreetNo, CT41.Street, CT41.Ward, CT41.District, CT41.CityID, AT02.CityName, CT41.[Description], CT41.[Disabled] 
+FROM CT0141 CT41 
+LEFT JOIN AT1002 AT02 ON AT02.DivisionID = CT41.DivisionID AND AT02.CityID = CT41.CityID
+WHERE CT41.DivisionID = @DivisionID
+ORDER BY CT41.StationID
+</t>
   </si>
 </sst>
 </file>
@@ -3200,6 +3208,9 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3227,9 +3238,6 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3299,6 +3307,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -3308,23 +3322,17 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3742,10 +3750,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="145"/>
+      <c r="B1" s="146"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -3772,8 +3780,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="145"/>
-      <c r="B2" s="145"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="146"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -3812,14 +3820,14 @@
       <c r="D4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="146" t="s">
+      <c r="E4" s="147" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="146"/>
-      <c r="G4" s="146"/>
-      <c r="H4" s="146"/>
-      <c r="I4" s="146"/>
-      <c r="J4" s="146"/>
+      <c r="F4" s="147"/>
+      <c r="G4" s="147"/>
+      <c r="H4" s="147"/>
+      <c r="I4" s="147"/>
+      <c r="J4" s="147"/>
     </row>
     <row r="5" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="40">
@@ -3834,14 +3842,14 @@
       <c r="D5" s="100" t="s">
         <v>231</v>
       </c>
-      <c r="E5" s="147" t="s">
+      <c r="E5" s="148" t="s">
         <v>232</v>
       </c>
-      <c r="F5" s="148"/>
-      <c r="G5" s="148"/>
-      <c r="H5" s="148"/>
-      <c r="I5" s="148"/>
-      <c r="J5" s="148"/>
+      <c r="F5" s="139"/>
+      <c r="G5" s="139"/>
+      <c r="H5" s="139"/>
+      <c r="I5" s="139"/>
+      <c r="J5" s="139"/>
     </row>
     <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="90">
@@ -3867,12 +3875,12 @@
       </c>
       <c r="C7" s="78"/>
       <c r="D7" s="40"/>
-      <c r="E7" s="139"/>
-      <c r="F7" s="140"/>
-      <c r="G7" s="140"/>
-      <c r="H7" s="140"/>
-      <c r="I7" s="140"/>
-      <c r="J7" s="141"/>
+      <c r="E7" s="140"/>
+      <c r="F7" s="141"/>
+      <c r="G7" s="141"/>
+      <c r="H7" s="141"/>
+      <c r="I7" s="141"/>
+      <c r="J7" s="142"/>
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="92">
@@ -3883,12 +3891,12 @@
       </c>
       <c r="C8" s="78"/>
       <c r="D8" s="40"/>
-      <c r="E8" s="142"/>
-      <c r="F8" s="143"/>
-      <c r="G8" s="143"/>
-      <c r="H8" s="143"/>
-      <c r="I8" s="143"/>
-      <c r="J8" s="144"/>
+      <c r="E8" s="143"/>
+      <c r="F8" s="144"/>
+      <c r="G8" s="144"/>
+      <c r="H8" s="144"/>
+      <c r="I8" s="144"/>
+      <c r="J8" s="145"/>
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="93">
@@ -3899,12 +3907,12 @@
       </c>
       <c r="C9" s="78"/>
       <c r="D9" s="40"/>
-      <c r="E9" s="139"/>
-      <c r="F9" s="140"/>
-      <c r="G9" s="140"/>
-      <c r="H9" s="140"/>
-      <c r="I9" s="140"/>
-      <c r="J9" s="141"/>
+      <c r="E9" s="140"/>
+      <c r="F9" s="141"/>
+      <c r="G9" s="141"/>
+      <c r="H9" s="141"/>
+      <c r="I9" s="141"/>
+      <c r="J9" s="142"/>
     </row>
     <row r="10" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="94">
@@ -3915,12 +3923,12 @@
       </c>
       <c r="C10" s="78"/>
       <c r="D10" s="40"/>
-      <c r="E10" s="139"/>
-      <c r="F10" s="140"/>
-      <c r="G10" s="140"/>
-      <c r="H10" s="140"/>
-      <c r="I10" s="140"/>
-      <c r="J10" s="141"/>
+      <c r="E10" s="140"/>
+      <c r="F10" s="141"/>
+      <c r="G10" s="141"/>
+      <c r="H10" s="141"/>
+      <c r="I10" s="141"/>
+      <c r="J10" s="142"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="95">
@@ -3931,12 +3939,12 @@
       </c>
       <c r="C11" s="78"/>
       <c r="D11" s="40"/>
-      <c r="E11" s="139"/>
-      <c r="F11" s="140"/>
-      <c r="G11" s="140"/>
-      <c r="H11" s="140"/>
-      <c r="I11" s="140"/>
-      <c r="J11" s="141"/>
+      <c r="E11" s="140"/>
+      <c r="F11" s="141"/>
+      <c r="G11" s="141"/>
+      <c r="H11" s="141"/>
+      <c r="I11" s="141"/>
+      <c r="J11" s="142"/>
     </row>
     <row r="12" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="96">
@@ -3947,12 +3955,12 @@
       </c>
       <c r="C12" s="78"/>
       <c r="D12" s="40"/>
-      <c r="E12" s="139"/>
-      <c r="F12" s="140"/>
-      <c r="G12" s="140"/>
-      <c r="H12" s="140"/>
-      <c r="I12" s="140"/>
-      <c r="J12" s="141"/>
+      <c r="E12" s="140"/>
+      <c r="F12" s="141"/>
+      <c r="G12" s="141"/>
+      <c r="H12" s="141"/>
+      <c r="I12" s="141"/>
+      <c r="J12" s="142"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="97">
@@ -3963,12 +3971,12 @@
       </c>
       <c r="C13" s="78"/>
       <c r="D13" s="40"/>
-      <c r="E13" s="139"/>
-      <c r="F13" s="140"/>
-      <c r="G13" s="140"/>
-      <c r="H13" s="140"/>
-      <c r="I13" s="140"/>
-      <c r="J13" s="141"/>
+      <c r="E13" s="140"/>
+      <c r="F13" s="141"/>
+      <c r="G13" s="141"/>
+      <c r="H13" s="141"/>
+      <c r="I13" s="141"/>
+      <c r="J13" s="142"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="98">
@@ -3979,12 +3987,12 @@
       </c>
       <c r="C14" s="78"/>
       <c r="D14" s="40"/>
-      <c r="E14" s="139"/>
-      <c r="F14" s="140"/>
-      <c r="G14" s="140"/>
-      <c r="H14" s="140"/>
-      <c r="I14" s="140"/>
-      <c r="J14" s="141"/>
+      <c r="E14" s="140"/>
+      <c r="F14" s="141"/>
+      <c r="G14" s="141"/>
+      <c r="H14" s="141"/>
+      <c r="I14" s="141"/>
+      <c r="J14" s="142"/>
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="40">
@@ -3995,12 +4003,12 @@
       </c>
       <c r="C15" s="78"/>
       <c r="D15" s="40"/>
-      <c r="E15" s="148"/>
-      <c r="F15" s="148"/>
-      <c r="G15" s="148"/>
-      <c r="H15" s="148"/>
-      <c r="I15" s="148"/>
-      <c r="J15" s="148"/>
+      <c r="E15" s="139"/>
+      <c r="F15" s="139"/>
+      <c r="G15" s="139"/>
+      <c r="H15" s="139"/>
+      <c r="I15" s="139"/>
+      <c r="J15" s="139"/>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="90">
@@ -4011,12 +4019,12 @@
       </c>
       <c r="C16" s="78"/>
       <c r="D16" s="40"/>
-      <c r="E16" s="148"/>
-      <c r="F16" s="148"/>
-      <c r="G16" s="148"/>
-      <c r="H16" s="148"/>
-      <c r="I16" s="148"/>
-      <c r="J16" s="148"/>
+      <c r="E16" s="139"/>
+      <c r="F16" s="139"/>
+      <c r="G16" s="139"/>
+      <c r="H16" s="139"/>
+      <c r="I16" s="139"/>
+      <c r="J16" s="139"/>
     </row>
     <row r="17" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="91">
@@ -4027,12 +4035,12 @@
       </c>
       <c r="C17" s="78"/>
       <c r="D17" s="40"/>
-      <c r="E17" s="148"/>
-      <c r="F17" s="148"/>
-      <c r="G17" s="148"/>
-      <c r="H17" s="148"/>
-      <c r="I17" s="148"/>
-      <c r="J17" s="148"/>
+      <c r="E17" s="139"/>
+      <c r="F17" s="139"/>
+      <c r="G17" s="139"/>
+      <c r="H17" s="139"/>
+      <c r="I17" s="139"/>
+      <c r="J17" s="139"/>
     </row>
     <row r="18" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="92">
@@ -4043,12 +4051,12 @@
       </c>
       <c r="C18" s="78"/>
       <c r="D18" s="40"/>
-      <c r="E18" s="148"/>
-      <c r="F18" s="148"/>
-      <c r="G18" s="148"/>
-      <c r="H18" s="148"/>
-      <c r="I18" s="148"/>
-      <c r="J18" s="148"/>
+      <c r="E18" s="139"/>
+      <c r="F18" s="139"/>
+      <c r="G18" s="139"/>
+      <c r="H18" s="139"/>
+      <c r="I18" s="139"/>
+      <c r="J18" s="139"/>
     </row>
     <row r="19" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="93">
@@ -4059,12 +4067,12 @@
       </c>
       <c r="C19" s="78"/>
       <c r="D19" s="40"/>
-      <c r="E19" s="148"/>
-      <c r="F19" s="148"/>
-      <c r="G19" s="148"/>
-      <c r="H19" s="148"/>
-      <c r="I19" s="148"/>
-      <c r="J19" s="148"/>
+      <c r="E19" s="139"/>
+      <c r="F19" s="139"/>
+      <c r="G19" s="139"/>
+      <c r="H19" s="139"/>
+      <c r="I19" s="139"/>
+      <c r="J19" s="139"/>
     </row>
     <row r="20" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="94">
@@ -4075,12 +4083,12 @@
       </c>
       <c r="C20" s="78"/>
       <c r="D20" s="40"/>
-      <c r="E20" s="148"/>
-      <c r="F20" s="148"/>
-      <c r="G20" s="148"/>
-      <c r="H20" s="148"/>
-      <c r="I20" s="148"/>
-      <c r="J20" s="148"/>
+      <c r="E20" s="139"/>
+      <c r="F20" s="139"/>
+      <c r="G20" s="139"/>
+      <c r="H20" s="139"/>
+      <c r="I20" s="139"/>
+      <c r="J20" s="139"/>
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="95">
@@ -4091,12 +4099,12 @@
       </c>
       <c r="C21" s="78"/>
       <c r="D21" s="40"/>
-      <c r="E21" s="148"/>
-      <c r="F21" s="148"/>
-      <c r="G21" s="148"/>
-      <c r="H21" s="148"/>
-      <c r="I21" s="148"/>
-      <c r="J21" s="148"/>
+      <c r="E21" s="139"/>
+      <c r="F21" s="139"/>
+      <c r="G21" s="139"/>
+      <c r="H21" s="139"/>
+      <c r="I21" s="139"/>
+      <c r="J21" s="139"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="96">
@@ -4107,12 +4115,12 @@
       </c>
       <c r="C22" s="78"/>
       <c r="D22" s="40"/>
-      <c r="E22" s="148"/>
-      <c r="F22" s="148"/>
-      <c r="G22" s="148"/>
-      <c r="H22" s="148"/>
-      <c r="I22" s="148"/>
-      <c r="J22" s="148"/>
+      <c r="E22" s="139"/>
+      <c r="F22" s="139"/>
+      <c r="G22" s="139"/>
+      <c r="H22" s="139"/>
+      <c r="I22" s="139"/>
+      <c r="J22" s="139"/>
     </row>
     <row r="23" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="97">
@@ -4123,12 +4131,12 @@
       </c>
       <c r="C23" s="78"/>
       <c r="D23" s="40"/>
-      <c r="E23" s="148"/>
-      <c r="F23" s="148"/>
-      <c r="G23" s="148"/>
-      <c r="H23" s="148"/>
-      <c r="I23" s="148"/>
-      <c r="J23" s="148"/>
+      <c r="E23" s="139"/>
+      <c r="F23" s="139"/>
+      <c r="G23" s="139"/>
+      <c r="H23" s="139"/>
+      <c r="I23" s="139"/>
+      <c r="J23" s="139"/>
     </row>
     <row r="24" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="98">
@@ -4139,12 +4147,12 @@
       </c>
       <c r="C24" s="78"/>
       <c r="D24" s="40"/>
-      <c r="E24" s="148"/>
-      <c r="F24" s="148"/>
-      <c r="G24" s="148"/>
-      <c r="H24" s="148"/>
-      <c r="I24" s="148"/>
-      <c r="J24" s="148"/>
+      <c r="E24" s="139"/>
+      <c r="F24" s="139"/>
+      <c r="G24" s="139"/>
+      <c r="H24" s="139"/>
+      <c r="I24" s="139"/>
+      <c r="J24" s="139"/>
     </row>
     <row r="25" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="40">
@@ -4155,12 +4163,12 @@
       </c>
       <c r="C25" s="78"/>
       <c r="D25" s="40"/>
-      <c r="E25" s="148"/>
-      <c r="F25" s="148"/>
-      <c r="G25" s="148"/>
-      <c r="H25" s="148"/>
-      <c r="I25" s="148"/>
-      <c r="J25" s="148"/>
+      <c r="E25" s="139"/>
+      <c r="F25" s="139"/>
+      <c r="G25" s="139"/>
+      <c r="H25" s="139"/>
+      <c r="I25" s="139"/>
+      <c r="J25" s="139"/>
     </row>
     <row r="26" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="90">
@@ -4171,12 +4179,12 @@
       </c>
       <c r="C26" s="78"/>
       <c r="D26" s="40"/>
-      <c r="E26" s="148"/>
-      <c r="F26" s="148"/>
-      <c r="G26" s="148"/>
-      <c r="H26" s="148"/>
-      <c r="I26" s="148"/>
-      <c r="J26" s="148"/>
+      <c r="E26" s="139"/>
+      <c r="F26" s="139"/>
+      <c r="G26" s="139"/>
+      <c r="H26" s="139"/>
+      <c r="I26" s="139"/>
+      <c r="J26" s="139"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="91">
@@ -4187,12 +4195,12 @@
       </c>
       <c r="C27" s="78"/>
       <c r="D27" s="40"/>
-      <c r="E27" s="148"/>
-      <c r="F27" s="148"/>
-      <c r="G27" s="148"/>
-      <c r="H27" s="148"/>
-      <c r="I27" s="148"/>
-      <c r="J27" s="148"/>
+      <c r="E27" s="139"/>
+      <c r="F27" s="139"/>
+      <c r="G27" s="139"/>
+      <c r="H27" s="139"/>
+      <c r="I27" s="139"/>
+      <c r="J27" s="139"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="92">
@@ -4203,12 +4211,12 @@
       </c>
       <c r="C28" s="78"/>
       <c r="D28" s="40"/>
-      <c r="E28" s="148"/>
-      <c r="F28" s="148"/>
-      <c r="G28" s="148"/>
-      <c r="H28" s="148"/>
-      <c r="I28" s="148"/>
-      <c r="J28" s="148"/>
+      <c r="E28" s="139"/>
+      <c r="F28" s="139"/>
+      <c r="G28" s="139"/>
+      <c r="H28" s="139"/>
+      <c r="I28" s="139"/>
+      <c r="J28" s="139"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="93">
@@ -4219,12 +4227,12 @@
       </c>
       <c r="C29" s="78"/>
       <c r="D29" s="40"/>
-      <c r="E29" s="148"/>
-      <c r="F29" s="148"/>
-      <c r="G29" s="148"/>
-      <c r="H29" s="148"/>
-      <c r="I29" s="148"/>
-      <c r="J29" s="148"/>
+      <c r="E29" s="139"/>
+      <c r="F29" s="139"/>
+      <c r="G29" s="139"/>
+      <c r="H29" s="139"/>
+      <c r="I29" s="139"/>
+      <c r="J29" s="139"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="94">
@@ -4235,12 +4243,12 @@
       </c>
       <c r="C30" s="78"/>
       <c r="D30" s="40"/>
-      <c r="E30" s="148"/>
-      <c r="F30" s="148"/>
-      <c r="G30" s="148"/>
-      <c r="H30" s="148"/>
-      <c r="I30" s="148"/>
-      <c r="J30" s="148"/>
+      <c r="E30" s="139"/>
+      <c r="F30" s="139"/>
+      <c r="G30" s="139"/>
+      <c r="H30" s="139"/>
+      <c r="I30" s="139"/>
+      <c r="J30" s="139"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="95">
@@ -4251,12 +4259,12 @@
       </c>
       <c r="C31" s="78"/>
       <c r="D31" s="40"/>
-      <c r="E31" s="148"/>
-      <c r="F31" s="148"/>
-      <c r="G31" s="148"/>
-      <c r="H31" s="148"/>
-      <c r="I31" s="148"/>
-      <c r="J31" s="148"/>
+      <c r="E31" s="139"/>
+      <c r="F31" s="139"/>
+      <c r="G31" s="139"/>
+      <c r="H31" s="139"/>
+      <c r="I31" s="139"/>
+      <c r="J31" s="139"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="96">
@@ -4267,12 +4275,12 @@
       </c>
       <c r="C32" s="78"/>
       <c r="D32" s="40"/>
-      <c r="E32" s="148"/>
-      <c r="F32" s="148"/>
-      <c r="G32" s="148"/>
-      <c r="H32" s="148"/>
-      <c r="I32" s="148"/>
-      <c r="J32" s="148"/>
+      <c r="E32" s="139"/>
+      <c r="F32" s="139"/>
+      <c r="G32" s="139"/>
+      <c r="H32" s="139"/>
+      <c r="I32" s="139"/>
+      <c r="J32" s="139"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="97">
@@ -4283,12 +4291,12 @@
       </c>
       <c r="C33" s="78"/>
       <c r="D33" s="40"/>
-      <c r="E33" s="148"/>
-      <c r="F33" s="148"/>
-      <c r="G33" s="148"/>
-      <c r="H33" s="148"/>
-      <c r="I33" s="148"/>
-      <c r="J33" s="148"/>
+      <c r="E33" s="139"/>
+      <c r="F33" s="139"/>
+      <c r="G33" s="139"/>
+      <c r="H33" s="139"/>
+      <c r="I33" s="139"/>
+      <c r="J33" s="139"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="98">
@@ -4299,12 +4307,12 @@
       </c>
       <c r="C34" s="78"/>
       <c r="D34" s="40"/>
-      <c r="E34" s="148"/>
-      <c r="F34" s="148"/>
-      <c r="G34" s="148"/>
-      <c r="H34" s="148"/>
-      <c r="I34" s="148"/>
-      <c r="J34" s="148"/>
+      <c r="E34" s="139"/>
+      <c r="F34" s="139"/>
+      <c r="G34" s="139"/>
+      <c r="H34" s="139"/>
+      <c r="I34" s="139"/>
+      <c r="J34" s="139"/>
     </row>
     <row r="35" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="40">
@@ -4315,12 +4323,12 @@
       </c>
       <c r="C35" s="78"/>
       <c r="D35" s="40"/>
-      <c r="E35" s="148"/>
-      <c r="F35" s="148"/>
-      <c r="G35" s="148"/>
-      <c r="H35" s="148"/>
-      <c r="I35" s="148"/>
-      <c r="J35" s="148"/>
+      <c r="E35" s="139"/>
+      <c r="F35" s="139"/>
+      <c r="G35" s="139"/>
+      <c r="H35" s="139"/>
+      <c r="I35" s="139"/>
+      <c r="J35" s="139"/>
     </row>
     <row r="36" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="90">
@@ -4331,12 +4339,12 @@
       </c>
       <c r="C36" s="78"/>
       <c r="D36" s="40"/>
-      <c r="E36" s="148"/>
-      <c r="F36" s="148"/>
-      <c r="G36" s="148"/>
-      <c r="H36" s="148"/>
-      <c r="I36" s="148"/>
-      <c r="J36" s="148"/>
+      <c r="E36" s="139"/>
+      <c r="F36" s="139"/>
+      <c r="G36" s="139"/>
+      <c r="H36" s="139"/>
+      <c r="I36" s="139"/>
+      <c r="J36" s="139"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="91">
@@ -4347,12 +4355,12 @@
       </c>
       <c r="C37" s="78"/>
       <c r="D37" s="40"/>
-      <c r="E37" s="148"/>
-      <c r="F37" s="148"/>
-      <c r="G37" s="148"/>
-      <c r="H37" s="148"/>
-      <c r="I37" s="148"/>
-      <c r="J37" s="148"/>
+      <c r="E37" s="139"/>
+      <c r="F37" s="139"/>
+      <c r="G37" s="139"/>
+      <c r="H37" s="139"/>
+      <c r="I37" s="139"/>
+      <c r="J37" s="139"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="92">
@@ -4363,12 +4371,12 @@
       </c>
       <c r="C38" s="78"/>
       <c r="D38" s="40"/>
-      <c r="E38" s="148"/>
-      <c r="F38" s="148"/>
-      <c r="G38" s="148"/>
-      <c r="H38" s="148"/>
-      <c r="I38" s="148"/>
-      <c r="J38" s="148"/>
+      <c r="E38" s="139"/>
+      <c r="F38" s="139"/>
+      <c r="G38" s="139"/>
+      <c r="H38" s="139"/>
+      <c r="I38" s="139"/>
+      <c r="J38" s="139"/>
     </row>
     <row r="39" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="93">
@@ -4379,12 +4387,12 @@
       </c>
       <c r="C39" s="78"/>
       <c r="D39" s="40"/>
-      <c r="E39" s="148"/>
-      <c r="F39" s="148"/>
-      <c r="G39" s="148"/>
-      <c r="H39" s="148"/>
-      <c r="I39" s="148"/>
-      <c r="J39" s="148"/>
+      <c r="E39" s="139"/>
+      <c r="F39" s="139"/>
+      <c r="G39" s="139"/>
+      <c r="H39" s="139"/>
+      <c r="I39" s="139"/>
+      <c r="J39" s="139"/>
     </row>
     <row r="40" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="94">
@@ -4395,12 +4403,12 @@
       </c>
       <c r="C40" s="78"/>
       <c r="D40" s="40"/>
-      <c r="E40" s="148"/>
-      <c r="F40" s="148"/>
-      <c r="G40" s="148"/>
-      <c r="H40" s="148"/>
-      <c r="I40" s="148"/>
-      <c r="J40" s="148"/>
+      <c r="E40" s="139"/>
+      <c r="F40" s="139"/>
+      <c r="G40" s="139"/>
+      <c r="H40" s="139"/>
+      <c r="I40" s="139"/>
+      <c r="J40" s="139"/>
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="95">
@@ -4411,12 +4419,12 @@
       </c>
       <c r="C41" s="78"/>
       <c r="D41" s="40"/>
-      <c r="E41" s="148"/>
-      <c r="F41" s="148"/>
-      <c r="G41" s="148"/>
-      <c r="H41" s="148"/>
-      <c r="I41" s="148"/>
-      <c r="J41" s="148"/>
+      <c r="E41" s="139"/>
+      <c r="F41" s="139"/>
+      <c r="G41" s="139"/>
+      <c r="H41" s="139"/>
+      <c r="I41" s="139"/>
+      <c r="J41" s="139"/>
     </row>
     <row r="42" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="96">
@@ -4427,32 +4435,23 @@
       </c>
       <c r="C42" s="78"/>
       <c r="D42" s="40"/>
-      <c r="E42" s="148"/>
-      <c r="F42" s="148"/>
-      <c r="G42" s="148"/>
-      <c r="H42" s="148"/>
-      <c r="I42" s="148"/>
-      <c r="J42" s="148"/>
+      <c r="E42" s="139"/>
+      <c r="F42" s="139"/>
+      <c r="G42" s="139"/>
+      <c r="H42" s="139"/>
+      <c r="I42" s="139"/>
+      <c r="J42" s="139"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="E38:J38"/>
-    <mergeCell ref="E39:J39"/>
-    <mergeCell ref="E40:J40"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E42:J42"/>
-    <mergeCell ref="E37:J37"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
     <mergeCell ref="E11:J11"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E25:J25"/>
@@ -4468,14 +4467,23 @@
     <mergeCell ref="E22:J22"/>
     <mergeCell ref="E23:J23"/>
     <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E42:J42"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
@@ -4692,10 +4700,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="145"/>
+      <c r="B1" s="146"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -4725,8 +4733,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="145"/>
-      <c r="B2" s="145"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="146"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -5302,13 +5310,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
       <c r="F1" s="30" t="s">
         <v>1</v>
       </c>
@@ -5341,11 +5349,11 @@
       </c>
     </row>
     <row r="2" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="145"/>
-      <c r="B2" s="145"/>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="146"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
       <c r="F2" s="30" t="s">
         <v>2</v>
       </c>
@@ -7751,7 +7759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -7776,7 +7784,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="172" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="129"/>
@@ -7809,7 +7817,7 @@
       <c r="L1" s="52"/>
     </row>
     <row r="2" spans="1:12" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="178"/>
+      <c r="A2" s="173"/>
       <c r="B2" s="130"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
@@ -7855,15 +7863,15 @@
       <c r="E4" s="101" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="145" t="s">
+      <c r="F4" s="146" t="s">
         <v>132</v>
       </c>
-      <c r="G4" s="145"/>
-      <c r="H4" s="145" t="s">
+      <c r="G4" s="146"/>
+      <c r="H4" s="146" t="s">
         <v>49</v>
       </c>
-      <c r="I4" s="145"/>
-      <c r="J4" s="145"/>
+      <c r="I4" s="146"/>
+      <c r="J4" s="146"/>
     </row>
     <row r="5" spans="1:12" s="34" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33">
@@ -7881,13 +7889,13 @@
       <c r="E5" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="F5" s="179" t="s">
+      <c r="F5" s="177" t="s">
         <v>250</v>
       </c>
-      <c r="G5" s="180"/>
-      <c r="H5" s="172"/>
-      <c r="I5" s="173"/>
-      <c r="J5" s="174"/>
+      <c r="G5" s="178"/>
+      <c r="H5" s="174"/>
+      <c r="I5" s="175"/>
+      <c r="J5" s="176"/>
     </row>
     <row r="6" spans="1:12" s="34" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A6" s="33">
@@ -7909,9 +7917,9 @@
         <v>251</v>
       </c>
       <c r="G6" s="182"/>
-      <c r="H6" s="172"/>
-      <c r="I6" s="173"/>
-      <c r="J6" s="174"/>
+      <c r="H6" s="174"/>
+      <c r="I6" s="175"/>
+      <c r="J6" s="176"/>
     </row>
     <row r="7" spans="1:12" s="34" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="33">
@@ -7933,9 +7941,9 @@
         <v>251</v>
       </c>
       <c r="G7" s="182"/>
-      <c r="H7" s="172"/>
-      <c r="I7" s="173"/>
-      <c r="J7" s="174"/>
+      <c r="H7" s="174"/>
+      <c r="I7" s="175"/>
+      <c r="J7" s="176"/>
     </row>
     <row r="8" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33">
@@ -7953,13 +7961,13 @@
       <c r="E8" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="F8" s="179" t="s">
+      <c r="F8" s="177" t="s">
         <v>245</v>
       </c>
-      <c r="G8" s="180"/>
-      <c r="H8" s="172"/>
-      <c r="I8" s="173"/>
-      <c r="J8" s="174"/>
+      <c r="G8" s="178"/>
+      <c r="H8" s="174"/>
+      <c r="I8" s="175"/>
+      <c r="J8" s="176"/>
     </row>
     <row r="9" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33">
@@ -7977,13 +7985,13 @@
       <c r="E9" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="F9" s="179" t="s">
+      <c r="F9" s="177" t="s">
         <v>247</v>
       </c>
-      <c r="G9" s="180"/>
-      <c r="H9" s="172"/>
-      <c r="I9" s="173"/>
-      <c r="J9" s="174"/>
+      <c r="G9" s="178"/>
+      <c r="H9" s="174"/>
+      <c r="I9" s="175"/>
+      <c r="J9" s="176"/>
     </row>
     <row r="10" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="33">
@@ -8001,13 +8009,13 @@
       <c r="E10" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="F10" s="179" t="s">
+      <c r="F10" s="177" t="s">
         <v>248</v>
       </c>
-      <c r="G10" s="180"/>
-      <c r="H10" s="172"/>
-      <c r="I10" s="173"/>
-      <c r="J10" s="174"/>
+      <c r="G10" s="178"/>
+      <c r="H10" s="174"/>
+      <c r="I10" s="175"/>
+      <c r="J10" s="176"/>
     </row>
     <row r="11" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="33">
@@ -8017,11 +8025,11 @@
       <c r="C11" s="33"/>
       <c r="D11" s="33"/>
       <c r="E11" s="32"/>
-      <c r="F11" s="175"/>
-      <c r="G11" s="176"/>
-      <c r="H11" s="172"/>
-      <c r="I11" s="173"/>
-      <c r="J11" s="174"/>
+      <c r="F11" s="179"/>
+      <c r="G11" s="180"/>
+      <c r="H11" s="174"/>
+      <c r="I11" s="175"/>
+      <c r="J11" s="176"/>
     </row>
     <row r="12" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="33">
@@ -8031,11 +8039,11 @@
       <c r="C12" s="33"/>
       <c r="D12" s="33"/>
       <c r="E12" s="32"/>
-      <c r="F12" s="175"/>
-      <c r="G12" s="176"/>
-      <c r="H12" s="172"/>
-      <c r="I12" s="173"/>
-      <c r="J12" s="174"/>
+      <c r="F12" s="179"/>
+      <c r="G12" s="180"/>
+      <c r="H12" s="174"/>
+      <c r="I12" s="175"/>
+      <c r="J12" s="176"/>
     </row>
     <row r="13" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33">
@@ -8045,11 +8053,11 @@
       <c r="C13" s="33"/>
       <c r="D13" s="33"/>
       <c r="E13" s="32"/>
-      <c r="F13" s="175"/>
-      <c r="G13" s="176"/>
-      <c r="H13" s="172"/>
-      <c r="I13" s="173"/>
-      <c r="J13" s="174"/>
+      <c r="F13" s="179"/>
+      <c r="G13" s="180"/>
+      <c r="H13" s="174"/>
+      <c r="I13" s="175"/>
+      <c r="J13" s="176"/>
     </row>
     <row r="14" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33">
@@ -8059,11 +8067,11 @@
       <c r="C14" s="33"/>
       <c r="D14" s="33"/>
       <c r="E14" s="32"/>
-      <c r="F14" s="175"/>
-      <c r="G14" s="176"/>
-      <c r="H14" s="172"/>
-      <c r="I14" s="173"/>
-      <c r="J14" s="174"/>
+      <c r="F14" s="179"/>
+      <c r="G14" s="180"/>
+      <c r="H14" s="174"/>
+      <c r="I14" s="175"/>
+      <c r="J14" s="176"/>
     </row>
     <row r="15" spans="1:12" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33">
@@ -8073,11 +8081,11 @@
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
       <c r="E15" s="32"/>
-      <c r="F15" s="175"/>
-      <c r="G15" s="176"/>
-      <c r="H15" s="172"/>
-      <c r="I15" s="173"/>
-      <c r="J15" s="174"/>
+      <c r="F15" s="179"/>
+      <c r="G15" s="180"/>
+      <c r="H15" s="174"/>
+      <c r="I15" s="175"/>
+      <c r="J15" s="176"/>
     </row>
     <row r="16" spans="1:12" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
       <c r="A16" s="33">
@@ -8087,11 +8095,11 @@
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>
       <c r="E16" s="32"/>
-      <c r="F16" s="175"/>
-      <c r="G16" s="176"/>
-      <c r="H16" s="172"/>
-      <c r="I16" s="173"/>
-      <c r="J16" s="174"/>
+      <c r="F16" s="179"/>
+      <c r="G16" s="180"/>
+      <c r="H16" s="174"/>
+      <c r="I16" s="175"/>
+      <c r="J16" s="176"/>
     </row>
     <row r="17" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="33">
@@ -8101,11 +8109,11 @@
       <c r="C17" s="33"/>
       <c r="D17" s="33"/>
       <c r="E17" s="32"/>
-      <c r="F17" s="175"/>
-      <c r="G17" s="176"/>
-      <c r="H17" s="172"/>
-      <c r="I17" s="173"/>
-      <c r="J17" s="174"/>
+      <c r="F17" s="179"/>
+      <c r="G17" s="180"/>
+      <c r="H17" s="174"/>
+      <c r="I17" s="175"/>
+      <c r="J17" s="176"/>
     </row>
     <row r="18" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="33">
@@ -8115,11 +8123,11 @@
       <c r="C18" s="33"/>
       <c r="D18" s="33"/>
       <c r="E18" s="32"/>
-      <c r="F18" s="175"/>
-      <c r="G18" s="176"/>
-      <c r="H18" s="172"/>
-      <c r="I18" s="173"/>
-      <c r="J18" s="174"/>
+      <c r="F18" s="179"/>
+      <c r="G18" s="180"/>
+      <c r="H18" s="174"/>
+      <c r="I18" s="175"/>
+      <c r="J18" s="176"/>
     </row>
     <row r="19" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="33">
@@ -8129,11 +8137,11 @@
       <c r="C19" s="33"/>
       <c r="D19" s="33"/>
       <c r="E19" s="32"/>
-      <c r="F19" s="175"/>
-      <c r="G19" s="176"/>
-      <c r="H19" s="172"/>
-      <c r="I19" s="173"/>
-      <c r="J19" s="174"/>
+      <c r="F19" s="179"/>
+      <c r="G19" s="180"/>
+      <c r="H19" s="174"/>
+      <c r="I19" s="175"/>
+      <c r="J19" s="176"/>
     </row>
     <row r="20" spans="1:18" s="34" customFormat="1" ht="11.25" x14ac:dyDescent="0.25">
       <c r="A20" s="33">
@@ -8143,11 +8151,11 @@
       <c r="C20" s="33"/>
       <c r="D20" s="33"/>
       <c r="E20" s="32"/>
-      <c r="F20" s="175"/>
-      <c r="G20" s="176"/>
-      <c r="H20" s="172"/>
-      <c r="I20" s="173"/>
-      <c r="J20" s="174"/>
+      <c r="F20" s="179"/>
+      <c r="G20" s="180"/>
+      <c r="H20" s="174"/>
+      <c r="I20" s="175"/>
+      <c r="J20" s="176"/>
     </row>
     <row r="21" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="33">
@@ -8157,11 +8165,11 @@
       <c r="C21" s="33"/>
       <c r="D21" s="33"/>
       <c r="E21" s="32"/>
-      <c r="F21" s="139"/>
-      <c r="G21" s="141"/>
-      <c r="H21" s="172"/>
-      <c r="I21" s="173"/>
-      <c r="J21" s="174"/>
+      <c r="F21" s="140"/>
+      <c r="G21" s="142"/>
+      <c r="H21" s="174"/>
+      <c r="I21" s="175"/>
+      <c r="J21" s="176"/>
     </row>
     <row r="22" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="33">
@@ -8171,11 +8179,11 @@
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
       <c r="E22" s="32"/>
-      <c r="F22" s="139"/>
-      <c r="G22" s="141"/>
-      <c r="H22" s="172"/>
-      <c r="I22" s="173"/>
-      <c r="J22" s="174"/>
+      <c r="F22" s="140"/>
+      <c r="G22" s="142"/>
+      <c r="H22" s="174"/>
+      <c r="I22" s="175"/>
+      <c r="J22" s="176"/>
     </row>
     <row r="23" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="33">
@@ -8185,11 +8193,11 @@
       <c r="C23" s="33"/>
       <c r="D23" s="33"/>
       <c r="E23" s="32"/>
-      <c r="F23" s="139"/>
-      <c r="G23" s="141"/>
-      <c r="H23" s="172"/>
-      <c r="I23" s="173"/>
-      <c r="J23" s="174"/>
+      <c r="F23" s="140"/>
+      <c r="G23" s="142"/>
+      <c r="H23" s="174"/>
+      <c r="I23" s="175"/>
+      <c r="J23" s="176"/>
     </row>
     <row r="24" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="33">
@@ -8199,11 +8207,11 @@
       <c r="C24" s="33"/>
       <c r="D24" s="33"/>
       <c r="E24" s="32"/>
-      <c r="F24" s="139"/>
-      <c r="G24" s="141"/>
-      <c r="H24" s="172"/>
-      <c r="I24" s="173"/>
-      <c r="J24" s="174"/>
+      <c r="F24" s="140"/>
+      <c r="G24" s="142"/>
+      <c r="H24" s="174"/>
+      <c r="I24" s="175"/>
+      <c r="J24" s="176"/>
     </row>
     <row r="25" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="33">
@@ -8213,11 +8221,11 @@
       <c r="C25" s="33"/>
       <c r="D25" s="33"/>
       <c r="E25" s="32"/>
-      <c r="F25" s="139"/>
-      <c r="G25" s="141"/>
-      <c r="H25" s="172"/>
-      <c r="I25" s="173"/>
-      <c r="J25" s="174"/>
+      <c r="F25" s="140"/>
+      <c r="G25" s="142"/>
+      <c r="H25" s="174"/>
+      <c r="I25" s="175"/>
+      <c r="J25" s="176"/>
     </row>
     <row r="26" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="33">
@@ -8227,11 +8235,11 @@
       <c r="C26" s="33"/>
       <c r="D26" s="33"/>
       <c r="E26" s="32"/>
-      <c r="F26" s="139"/>
-      <c r="G26" s="141"/>
-      <c r="H26" s="172"/>
-      <c r="I26" s="173"/>
-      <c r="J26" s="174"/>
+      <c r="F26" s="140"/>
+      <c r="G26" s="142"/>
+      <c r="H26" s="174"/>
+      <c r="I26" s="175"/>
+      <c r="J26" s="176"/>
     </row>
     <row r="27" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="33">
@@ -8241,11 +8249,11 @@
       <c r="C27" s="33"/>
       <c r="D27" s="33"/>
       <c r="E27" s="32"/>
-      <c r="F27" s="139"/>
-      <c r="G27" s="141"/>
-      <c r="H27" s="172"/>
-      <c r="I27" s="173"/>
-      <c r="J27" s="174"/>
+      <c r="F27" s="140"/>
+      <c r="G27" s="142"/>
+      <c r="H27" s="174"/>
+      <c r="I27" s="175"/>
+      <c r="J27" s="176"/>
     </row>
     <row r="28" spans="1:18" s="34" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="33">
@@ -8255,11 +8263,11 @@
       <c r="C28" s="33"/>
       <c r="D28" s="33"/>
       <c r="E28" s="32"/>
-      <c r="F28" s="139"/>
-      <c r="G28" s="141"/>
-      <c r="H28" s="172"/>
-      <c r="I28" s="173"/>
-      <c r="J28" s="174"/>
+      <c r="F28" s="140"/>
+      <c r="G28" s="142"/>
+      <c r="H28" s="174"/>
+      <c r="I28" s="175"/>
+      <c r="J28" s="176"/>
     </row>
     <row r="29" spans="1:18" s="34" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="33">
@@ -8269,11 +8277,11 @@
       <c r="C29" s="33"/>
       <c r="D29" s="33"/>
       <c r="E29" s="32"/>
-      <c r="F29" s="139"/>
-      <c r="G29" s="141"/>
-      <c r="H29" s="172"/>
-      <c r="I29" s="173"/>
-      <c r="J29" s="174"/>
+      <c r="F29" s="140"/>
+      <c r="G29" s="142"/>
+      <c r="H29" s="174"/>
+      <c r="I29" s="175"/>
+      <c r="J29" s="176"/>
     </row>
     <row r="30" spans="1:18" s="34" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="33">
@@ -8283,11 +8291,11 @@
       <c r="C30" s="33"/>
       <c r="D30" s="33"/>
       <c r="E30" s="32"/>
-      <c r="F30" s="139"/>
-      <c r="G30" s="141"/>
-      <c r="H30" s="172"/>
-      <c r="I30" s="173"/>
-      <c r="J30" s="174"/>
+      <c r="F30" s="140"/>
+      <c r="G30" s="142"/>
+      <c r="H30" s="174"/>
+      <c r="I30" s="175"/>
+      <c r="J30" s="176"/>
     </row>
     <row r="31" spans="1:18" ht="11.25" x14ac:dyDescent="0.15">
       <c r="A31" s="33">
@@ -8297,11 +8305,11 @@
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
       <c r="E31" s="32"/>
-      <c r="F31" s="139"/>
-      <c r="G31" s="141"/>
-      <c r="H31" s="172"/>
-      <c r="I31" s="173"/>
-      <c r="J31" s="174"/>
+      <c r="F31" s="140"/>
+      <c r="G31" s="142"/>
+      <c r="H31" s="174"/>
+      <c r="I31" s="175"/>
+      <c r="J31" s="176"/>
       <c r="L31" s="22"/>
       <c r="M31" s="22"/>
       <c r="N31" s="22"/>
@@ -8318,11 +8326,11 @@
       <c r="C32" s="33"/>
       <c r="D32" s="33"/>
       <c r="E32" s="32"/>
-      <c r="F32" s="139"/>
-      <c r="G32" s="141"/>
-      <c r="H32" s="172"/>
-      <c r="I32" s="173"/>
-      <c r="J32" s="174"/>
+      <c r="F32" s="140"/>
+      <c r="G32" s="142"/>
+      <c r="H32" s="174"/>
+      <c r="I32" s="175"/>
+      <c r="J32" s="176"/>
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
       <c r="N32" s="22"/>
@@ -8339,11 +8347,11 @@
       <c r="C33" s="33"/>
       <c r="D33" s="33"/>
       <c r="E33" s="32"/>
-      <c r="F33" s="139"/>
-      <c r="G33" s="141"/>
-      <c r="H33" s="172"/>
-      <c r="I33" s="173"/>
-      <c r="J33" s="174"/>
+      <c r="F33" s="140"/>
+      <c r="G33" s="142"/>
+      <c r="H33" s="174"/>
+      <c r="I33" s="175"/>
+      <c r="J33" s="176"/>
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
       <c r="N33" s="22"/>
@@ -8360,11 +8368,11 @@
       <c r="C34" s="33"/>
       <c r="D34" s="33"/>
       <c r="E34" s="32"/>
-      <c r="F34" s="139"/>
-      <c r="G34" s="141"/>
-      <c r="H34" s="172"/>
-      <c r="I34" s="173"/>
-      <c r="J34" s="174"/>
+      <c r="F34" s="140"/>
+      <c r="G34" s="142"/>
+      <c r="H34" s="174"/>
+      <c r="I34" s="175"/>
+      <c r="J34" s="176"/>
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
       <c r="N34" s="22"/>
@@ -8381,11 +8389,11 @@
       <c r="C35" s="33"/>
       <c r="D35" s="33"/>
       <c r="E35" s="32"/>
-      <c r="F35" s="139"/>
-      <c r="G35" s="141"/>
-      <c r="H35" s="172"/>
-      <c r="I35" s="173"/>
-      <c r="J35" s="174"/>
+      <c r="F35" s="140"/>
+      <c r="G35" s="142"/>
+      <c r="H35" s="174"/>
+      <c r="I35" s="175"/>
+      <c r="J35" s="176"/>
       <c r="L35" s="22"/>
       <c r="M35" s="22"/>
       <c r="N35" s="22"/>
@@ -8402,11 +8410,11 @@
       <c r="C36" s="33"/>
       <c r="D36" s="33"/>
       <c r="E36" s="32"/>
-      <c r="F36" s="139"/>
-      <c r="G36" s="141"/>
-      <c r="H36" s="172"/>
-      <c r="I36" s="173"/>
-      <c r="J36" s="174"/>
+      <c r="F36" s="140"/>
+      <c r="G36" s="142"/>
+      <c r="H36" s="174"/>
+      <c r="I36" s="175"/>
+      <c r="J36" s="176"/>
       <c r="L36" s="22"/>
       <c r="M36" s="22"/>
       <c r="N36" s="22"/>
@@ -8423,11 +8431,11 @@
       <c r="C37" s="33"/>
       <c r="D37" s="33"/>
       <c r="E37" s="32"/>
-      <c r="F37" s="139"/>
-      <c r="G37" s="141"/>
-      <c r="H37" s="172"/>
-      <c r="I37" s="173"/>
-      <c r="J37" s="174"/>
+      <c r="F37" s="140"/>
+      <c r="G37" s="142"/>
+      <c r="H37" s="174"/>
+      <c r="I37" s="175"/>
+      <c r="J37" s="176"/>
       <c r="L37" s="22"/>
       <c r="M37" s="22"/>
       <c r="N37" s="22"/>
@@ -8444,11 +8452,11 @@
       <c r="C38" s="33"/>
       <c r="D38" s="33"/>
       <c r="E38" s="32"/>
-      <c r="F38" s="139"/>
-      <c r="G38" s="141"/>
-      <c r="H38" s="172"/>
-      <c r="I38" s="173"/>
-      <c r="J38" s="174"/>
+      <c r="F38" s="140"/>
+      <c r="G38" s="142"/>
+      <c r="H38" s="174"/>
+      <c r="I38" s="175"/>
+      <c r="J38" s="176"/>
       <c r="L38" s="22"/>
       <c r="M38" s="22"/>
       <c r="N38" s="22"/>
@@ -8465,11 +8473,11 @@
       <c r="C39" s="33"/>
       <c r="D39" s="33"/>
       <c r="E39" s="32"/>
-      <c r="F39" s="139"/>
-      <c r="G39" s="141"/>
-      <c r="H39" s="172"/>
-      <c r="I39" s="173"/>
-      <c r="J39" s="174"/>
+      <c r="F39" s="140"/>
+      <c r="G39" s="142"/>
+      <c r="H39" s="174"/>
+      <c r="I39" s="175"/>
+      <c r="J39" s="176"/>
       <c r="L39" s="22"/>
       <c r="M39" s="22"/>
       <c r="N39" s="22"/>
@@ -8486,11 +8494,11 @@
       <c r="C40" s="33"/>
       <c r="D40" s="33"/>
       <c r="E40" s="32"/>
-      <c r="F40" s="139"/>
-      <c r="G40" s="141"/>
-      <c r="H40" s="172"/>
-      <c r="I40" s="173"/>
-      <c r="J40" s="174"/>
+      <c r="F40" s="140"/>
+      <c r="G40" s="142"/>
+      <c r="H40" s="174"/>
+      <c r="I40" s="175"/>
+      <c r="J40" s="176"/>
       <c r="L40" s="22"/>
       <c r="M40" s="22"/>
       <c r="N40" s="22"/>
@@ -8507,11 +8515,11 @@
       <c r="C41" s="33"/>
       <c r="D41" s="33"/>
       <c r="E41" s="32"/>
-      <c r="F41" s="139"/>
-      <c r="G41" s="141"/>
-      <c r="H41" s="172"/>
-      <c r="I41" s="173"/>
-      <c r="J41" s="174"/>
+      <c r="F41" s="140"/>
+      <c r="G41" s="142"/>
+      <c r="H41" s="174"/>
+      <c r="I41" s="175"/>
+      <c r="J41" s="176"/>
       <c r="L41" s="22"/>
       <c r="M41" s="22"/>
       <c r="N41" s="22"/>
@@ -8528,11 +8536,11 @@
       <c r="C42" s="33"/>
       <c r="D42" s="33"/>
       <c r="E42" s="32"/>
-      <c r="F42" s="139"/>
-      <c r="G42" s="141"/>
-      <c r="H42" s="172"/>
-      <c r="I42" s="173"/>
-      <c r="J42" s="174"/>
+      <c r="F42" s="140"/>
+      <c r="G42" s="142"/>
+      <c r="H42" s="174"/>
+      <c r="I42" s="175"/>
+      <c r="J42" s="176"/>
       <c r="L42" s="22"/>
       <c r="M42" s="22"/>
       <c r="N42" s="22"/>
@@ -8549,11 +8557,11 @@
       <c r="C43" s="33"/>
       <c r="D43" s="33"/>
       <c r="E43" s="32"/>
-      <c r="F43" s="139"/>
-      <c r="G43" s="141"/>
-      <c r="H43" s="172"/>
-      <c r="I43" s="173"/>
-      <c r="J43" s="174"/>
+      <c r="F43" s="140"/>
+      <c r="G43" s="142"/>
+      <c r="H43" s="174"/>
+      <c r="I43" s="175"/>
+      <c r="J43" s="176"/>
       <c r="L43" s="22"/>
       <c r="M43" s="22"/>
       <c r="N43" s="22"/>
@@ -8570,11 +8578,11 @@
       <c r="C44" s="33"/>
       <c r="D44" s="33"/>
       <c r="E44" s="32"/>
-      <c r="F44" s="139"/>
-      <c r="G44" s="141"/>
-      <c r="H44" s="172"/>
-      <c r="I44" s="173"/>
-      <c r="J44" s="174"/>
+      <c r="F44" s="140"/>
+      <c r="G44" s="142"/>
+      <c r="H44" s="174"/>
+      <c r="I44" s="175"/>
+      <c r="J44" s="176"/>
       <c r="L44" s="22"/>
       <c r="M44" s="22"/>
       <c r="N44" s="22"/>
@@ -8591,11 +8599,11 @@
       <c r="C45" s="33"/>
       <c r="D45" s="33"/>
       <c r="E45" s="32"/>
-      <c r="F45" s="139"/>
-      <c r="G45" s="141"/>
-      <c r="H45" s="172"/>
-      <c r="I45" s="173"/>
-      <c r="J45" s="174"/>
+      <c r="F45" s="140"/>
+      <c r="G45" s="142"/>
+      <c r="H45" s="174"/>
+      <c r="I45" s="175"/>
+      <c r="J45" s="176"/>
       <c r="L45" s="22"/>
       <c r="M45" s="22"/>
       <c r="N45" s="22"/>
@@ -8612,11 +8620,11 @@
       <c r="C46" s="33"/>
       <c r="D46" s="33"/>
       <c r="E46" s="32"/>
-      <c r="F46" s="139"/>
-      <c r="G46" s="141"/>
-      <c r="H46" s="172"/>
-      <c r="I46" s="173"/>
-      <c r="J46" s="174"/>
+      <c r="F46" s="140"/>
+      <c r="G46" s="142"/>
+      <c r="H46" s="174"/>
+      <c r="I46" s="175"/>
+      <c r="J46" s="176"/>
       <c r="L46" s="22"/>
       <c r="M46" s="22"/>
       <c r="N46" s="22"/>
@@ -8633,11 +8641,11 @@
       <c r="C47" s="33"/>
       <c r="D47" s="33"/>
       <c r="E47" s="32"/>
-      <c r="F47" s="139"/>
-      <c r="G47" s="141"/>
-      <c r="H47" s="172"/>
-      <c r="I47" s="173"/>
-      <c r="J47" s="174"/>
+      <c r="F47" s="140"/>
+      <c r="G47" s="142"/>
+      <c r="H47" s="174"/>
+      <c r="I47" s="175"/>
+      <c r="J47" s="176"/>
       <c r="L47" s="22"/>
       <c r="M47" s="22"/>
       <c r="N47" s="22"/>
@@ -8654,11 +8662,11 @@
       <c r="C48" s="33"/>
       <c r="D48" s="33"/>
       <c r="E48" s="32"/>
-      <c r="F48" s="139"/>
-      <c r="G48" s="141"/>
-      <c r="H48" s="172"/>
-      <c r="I48" s="173"/>
-      <c r="J48" s="174"/>
+      <c r="F48" s="140"/>
+      <c r="G48" s="142"/>
+      <c r="H48" s="174"/>
+      <c r="I48" s="175"/>
+      <c r="J48" s="176"/>
       <c r="L48" s="22"/>
       <c r="M48" s="22"/>
       <c r="N48" s="22"/>
@@ -8675,11 +8683,11 @@
       <c r="C49" s="33"/>
       <c r="D49" s="33"/>
       <c r="E49" s="32"/>
-      <c r="F49" s="139"/>
-      <c r="G49" s="141"/>
-      <c r="H49" s="172"/>
-      <c r="I49" s="173"/>
-      <c r="J49" s="174"/>
+      <c r="F49" s="140"/>
+      <c r="G49" s="142"/>
+      <c r="H49" s="174"/>
+      <c r="I49" s="175"/>
+      <c r="J49" s="176"/>
       <c r="L49" s="22"/>
       <c r="M49" s="22"/>
       <c r="N49" s="22"/>
@@ -8696,11 +8704,11 @@
       <c r="C50" s="33"/>
       <c r="D50" s="33"/>
       <c r="E50" s="32"/>
-      <c r="F50" s="139"/>
-      <c r="G50" s="141"/>
-      <c r="H50" s="172"/>
-      <c r="I50" s="173"/>
-      <c r="J50" s="174"/>
+      <c r="F50" s="140"/>
+      <c r="G50" s="142"/>
+      <c r="H50" s="174"/>
+      <c r="I50" s="175"/>
+      <c r="J50" s="176"/>
       <c r="L50" s="22"/>
       <c r="M50" s="22"/>
       <c r="N50" s="22"/>
@@ -8717,11 +8725,11 @@
       <c r="C51" s="33"/>
       <c r="D51" s="33"/>
       <c r="E51" s="32"/>
-      <c r="F51" s="139"/>
-      <c r="G51" s="141"/>
-      <c r="H51" s="172"/>
-      <c r="I51" s="173"/>
-      <c r="J51" s="174"/>
+      <c r="F51" s="140"/>
+      <c r="G51" s="142"/>
+      <c r="H51" s="174"/>
+      <c r="I51" s="175"/>
+      <c r="J51" s="176"/>
       <c r="L51" s="22"/>
       <c r="M51" s="22"/>
       <c r="N51" s="22"/>
@@ -8738,11 +8746,11 @@
       <c r="C52" s="33"/>
       <c r="D52" s="33"/>
       <c r="E52" s="32"/>
-      <c r="F52" s="139"/>
-      <c r="G52" s="141"/>
-      <c r="H52" s="172"/>
-      <c r="I52" s="173"/>
-      <c r="J52" s="174"/>
+      <c r="F52" s="140"/>
+      <c r="G52" s="142"/>
+      <c r="H52" s="174"/>
+      <c r="I52" s="175"/>
+      <c r="J52" s="176"/>
       <c r="L52" s="22"/>
       <c r="M52" s="22"/>
       <c r="N52" s="22"/>
@@ -8759,11 +8767,11 @@
       <c r="C53" s="33"/>
       <c r="D53" s="33"/>
       <c r="E53" s="32"/>
-      <c r="F53" s="139"/>
-      <c r="G53" s="141"/>
-      <c r="H53" s="172"/>
-      <c r="I53" s="173"/>
-      <c r="J53" s="174"/>
+      <c r="F53" s="140"/>
+      <c r="G53" s="142"/>
+      <c r="H53" s="174"/>
+      <c r="I53" s="175"/>
+      <c r="J53" s="176"/>
       <c r="L53" s="22"/>
       <c r="M53" s="22"/>
       <c r="N53" s="22"/>
@@ -8780,11 +8788,11 @@
       <c r="C54" s="33"/>
       <c r="D54" s="33"/>
       <c r="E54" s="32"/>
-      <c r="F54" s="139"/>
-      <c r="G54" s="141"/>
-      <c r="H54" s="172"/>
-      <c r="I54" s="173"/>
-      <c r="J54" s="174"/>
+      <c r="F54" s="140"/>
+      <c r="G54" s="142"/>
+      <c r="H54" s="174"/>
+      <c r="I54" s="175"/>
+      <c r="J54" s="176"/>
       <c r="L54" s="22"/>
       <c r="M54" s="22"/>
       <c r="N54" s="22"/>
@@ -8801,11 +8809,11 @@
       <c r="C55" s="33"/>
       <c r="D55" s="33"/>
       <c r="E55" s="32"/>
-      <c r="F55" s="139"/>
-      <c r="G55" s="141"/>
-      <c r="H55" s="172"/>
-      <c r="I55" s="173"/>
-      <c r="J55" s="174"/>
+      <c r="F55" s="140"/>
+      <c r="G55" s="142"/>
+      <c r="H55" s="174"/>
+      <c r="I55" s="175"/>
+      <c r="J55" s="176"/>
       <c r="L55" s="22"/>
       <c r="M55" s="22"/>
       <c r="N55" s="22"/>
@@ -8817,6 +8825,94 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="105">
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="H49:J49"/>
+    <mergeCell ref="H50:J50"/>
+    <mergeCell ref="H51:J51"/>
+    <mergeCell ref="H52:J52"/>
+    <mergeCell ref="H53:J53"/>
+    <mergeCell ref="H54:J54"/>
+    <mergeCell ref="H55:J55"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="H48:J48"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H37:J37"/>
+    <mergeCell ref="H38:J38"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="H41:J41"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="H31:J31"/>
+    <mergeCell ref="H32:J32"/>
+    <mergeCell ref="H33:J33"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="H35:J35"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="H28:J28"/>
+    <mergeCell ref="H29:J29"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="H23:J23"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="H18:J18"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="H6:J6"/>
@@ -8834,94 +8930,6 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="H23:J23"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H25:J25"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="H27:J27"/>
-    <mergeCell ref="H28:J28"/>
-    <mergeCell ref="H29:J29"/>
-    <mergeCell ref="H30:J30"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="H31:J31"/>
-    <mergeCell ref="H32:J32"/>
-    <mergeCell ref="H33:J33"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="H35:J35"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H37:J37"/>
-    <mergeCell ref="H38:J38"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="H41:J41"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="H48:J48"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="H49:J49"/>
-    <mergeCell ref="H50:J50"/>
-    <mergeCell ref="H51:J51"/>
-    <mergeCell ref="H52:J52"/>
-    <mergeCell ref="H53:J53"/>
-    <mergeCell ref="H54:J54"/>
-    <mergeCell ref="H55:J55"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E55">
@@ -8943,8 +8951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1048467"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8972,16 +8980,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="145"/>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
       <c r="I1" s="31" t="s">
         <v>1</v>
       </c>
@@ -9016,14 +9024,14 @@
       <c r="U1" s="52"/>
     </row>
     <row r="2" spans="1:21" s="25" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="145"/>
-      <c r="B2" s="145"/>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
-      <c r="F2" s="145"/>
-      <c r="G2" s="145"/>
-      <c r="H2" s="145"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="146"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="146"/>
       <c r="I2" s="31" t="s">
         <v>2</v>
       </c>
@@ -9141,6 +9149,12 @@
       <c r="J5" s="123" t="s">
         <v>220</v>
       </c>
+      <c r="K5" s="143" t="s">
+        <v>292</v>
+      </c>
+      <c r="L5" s="144"/>
+      <c r="M5" s="144"/>
+      <c r="N5" s="145"/>
       <c r="O5" s="127" t="s">
         <v>135</v>
       </c>
@@ -9184,12 +9198,12 @@
       <c r="J6" s="123" t="s">
         <v>221</v>
       </c>
-      <c r="K6" s="142" t="s">
+      <c r="K6" s="143" t="s">
         <v>261</v>
       </c>
-      <c r="L6" s="143"/>
-      <c r="M6" s="143"/>
-      <c r="N6" s="144"/>
+      <c r="L6" s="144"/>
+      <c r="M6" s="144"/>
+      <c r="N6" s="145"/>
       <c r="O6" s="121" t="s">
         <v>228</v>
       </c>
@@ -9235,12 +9249,12 @@
       <c r="J7" s="123" t="s">
         <v>222</v>
       </c>
-      <c r="K7" s="142" t="s">
+      <c r="K7" s="143" t="s">
         <v>264</v>
       </c>
-      <c r="L7" s="143"/>
-      <c r="M7" s="143"/>
-      <c r="N7" s="144"/>
+      <c r="L7" s="144"/>
+      <c r="M7" s="144"/>
+      <c r="N7" s="145"/>
       <c r="O7" s="121" t="s">
         <v>223</v>
       </c>
@@ -11377,33 +11391,59 @@
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="93">
-    <mergeCell ref="K88:N88"/>
-    <mergeCell ref="K89:N89"/>
-    <mergeCell ref="K90:N90"/>
-    <mergeCell ref="K91:N91"/>
-    <mergeCell ref="K92:N92"/>
-    <mergeCell ref="K77:N77"/>
-    <mergeCell ref="K60:N60"/>
-    <mergeCell ref="K87:N87"/>
-    <mergeCell ref="K61:N61"/>
-    <mergeCell ref="K62:N62"/>
-    <mergeCell ref="K63:N63"/>
-    <mergeCell ref="K64:N64"/>
-    <mergeCell ref="K65:N65"/>
-    <mergeCell ref="K66:N66"/>
-    <mergeCell ref="K67:N67"/>
-    <mergeCell ref="K68:N68"/>
-    <mergeCell ref="K74:N74"/>
-    <mergeCell ref="K75:N75"/>
-    <mergeCell ref="K76:N76"/>
-    <mergeCell ref="K53:N53"/>
-    <mergeCell ref="K72:N72"/>
-    <mergeCell ref="K73:N73"/>
-    <mergeCell ref="K59:N59"/>
-    <mergeCell ref="K55:N55"/>
-    <mergeCell ref="K56:N56"/>
-    <mergeCell ref="K57:N57"/>
+  <mergeCells count="94">
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="K13:N13"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="K23:N23"/>
+    <mergeCell ref="K24:N24"/>
+    <mergeCell ref="K25:N25"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="K27:N27"/>
+    <mergeCell ref="K28:N28"/>
+    <mergeCell ref="K29:N29"/>
+    <mergeCell ref="K30:N30"/>
+    <mergeCell ref="K31:N31"/>
+    <mergeCell ref="K32:N32"/>
+    <mergeCell ref="K33:N33"/>
+    <mergeCell ref="K34:N34"/>
+    <mergeCell ref="K35:N35"/>
+    <mergeCell ref="K36:N36"/>
+    <mergeCell ref="K37:N37"/>
+    <mergeCell ref="K39:N39"/>
+    <mergeCell ref="K40:N40"/>
+    <mergeCell ref="K41:N41"/>
+    <mergeCell ref="K58:N58"/>
+    <mergeCell ref="K47:N47"/>
+    <mergeCell ref="K48:N48"/>
+    <mergeCell ref="K49:N49"/>
+    <mergeCell ref="K50:N50"/>
+    <mergeCell ref="K54:N54"/>
+    <mergeCell ref="K42:N42"/>
+    <mergeCell ref="K43:N43"/>
+    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="K45:N45"/>
+    <mergeCell ref="K46:N46"/>
+    <mergeCell ref="K51:N51"/>
+    <mergeCell ref="K52:N52"/>
     <mergeCell ref="K93:N93"/>
     <mergeCell ref="K94:N94"/>
     <mergeCell ref="K6:N6"/>
@@ -11420,57 +11460,32 @@
     <mergeCell ref="K70:N70"/>
     <mergeCell ref="K71:N71"/>
     <mergeCell ref="K38:N38"/>
-    <mergeCell ref="K39:N39"/>
-    <mergeCell ref="K40:N40"/>
-    <mergeCell ref="K41:N41"/>
-    <mergeCell ref="K58:N58"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="K48:N48"/>
-    <mergeCell ref="K49:N49"/>
-    <mergeCell ref="K50:N50"/>
-    <mergeCell ref="K54:N54"/>
-    <mergeCell ref="K42:N42"/>
-    <mergeCell ref="K43:N43"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="K45:N45"/>
-    <mergeCell ref="K46:N46"/>
-    <mergeCell ref="K51:N51"/>
-    <mergeCell ref="K52:N52"/>
-    <mergeCell ref="K33:N33"/>
-    <mergeCell ref="K34:N34"/>
-    <mergeCell ref="K35:N35"/>
-    <mergeCell ref="K36:N36"/>
-    <mergeCell ref="K37:N37"/>
-    <mergeCell ref="K28:N28"/>
-    <mergeCell ref="K29:N29"/>
-    <mergeCell ref="K30:N30"/>
-    <mergeCell ref="K31:N31"/>
-    <mergeCell ref="K32:N32"/>
-    <mergeCell ref="K23:N23"/>
-    <mergeCell ref="K24:N24"/>
-    <mergeCell ref="K25:N25"/>
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="K27:N27"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="K19:N19"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="K17:N17"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="K53:N53"/>
+    <mergeCell ref="K72:N72"/>
+    <mergeCell ref="K73:N73"/>
+    <mergeCell ref="K59:N59"/>
+    <mergeCell ref="K55:N55"/>
+    <mergeCell ref="K56:N56"/>
+    <mergeCell ref="K57:N57"/>
+    <mergeCell ref="K77:N77"/>
+    <mergeCell ref="K60:N60"/>
+    <mergeCell ref="K87:N87"/>
+    <mergeCell ref="K61:N61"/>
+    <mergeCell ref="K62:N62"/>
+    <mergeCell ref="K63:N63"/>
+    <mergeCell ref="K64:N64"/>
+    <mergeCell ref="K65:N65"/>
+    <mergeCell ref="K66:N66"/>
+    <mergeCell ref="K67:N67"/>
+    <mergeCell ref="K68:N68"/>
+    <mergeCell ref="K74:N74"/>
+    <mergeCell ref="K75:N75"/>
+    <mergeCell ref="K76:N76"/>
+    <mergeCell ref="K88:N88"/>
+    <mergeCell ref="K89:N89"/>
+    <mergeCell ref="K90:N90"/>
+    <mergeCell ref="K91:N91"/>
+    <mergeCell ref="K92:N92"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="Q1048467:Q1048576 Q5:Q94"/>
@@ -11516,10 +11531,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="145"/>
+      <c r="B1" s="146"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -11549,8 +11564,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="145"/>
-      <c r="B2" s="145"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="146"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -12845,10 +12860,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="145" t="s">
+      <c r="A1" s="146" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="145"/>
+      <c r="B1" s="146"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -12876,8 +12891,8 @@
       <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="145"/>
-      <c r="B2" s="145"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="146"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>

</xml_diff>